<commit_message>
Update AgID- SDG OOTS_ListaUtenzeDiTest_v01.xlsx
</commit_message>
<xml_diff>
--- a/SDG - Componenti Nazionali/AgID- SDG OOTS_ListaUtenzeDiTest_v01.xlsx
+++ b/SDG - Componenti Nazionali/AgID- SDG OOTS_ListaUtenzeDiTest_v01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francesco.pitarresi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCF15D8-5D70-4E96-9031-72FC7E065730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5E9275-0D78-4328-9489-DA985ACAD2C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{57EAA282-3640-4213-9366-C1200017E5D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{57EAA282-3640-4213-9366-C1200017E5D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>ROMA</t>
   </si>
   <si>
-    <t>CERTIFICATO</t>
-  </si>
-  <si>
     <t>202312345003</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
     <t>STATI UNITI AMERICA</t>
   </si>
   <si>
-    <t>TESSERINO</t>
-  </si>
-  <si>
     <t>3550000011</t>
   </si>
   <si>
@@ -240,6 +234,12 @@
   </si>
   <si>
     <t>05/04/1981</t>
+  </si>
+  <si>
+    <t>certificato</t>
+  </si>
+  <si>
+    <t>tesserino</t>
   </si>
 </sst>
 </file>
@@ -689,26 +689,26 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.81640625" customWidth="1"/>
-    <col min="11" max="11" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
     <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="71.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" ht="71.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -743,13 +743,13 @@
         <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>11</v>
       </c>
@@ -773,36 +773,36 @@
         <v>17</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="6" t="s">
@@ -812,36 +812,36 @@
         <v>17</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="6" t="s">
@@ -851,147 +851,147 @@
         <v>17</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="J4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="B5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G5" s="6"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="L5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="G6" s="6"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>23</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="J7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="B8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="L7" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>49</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="6" t="s">
@@ -1001,96 +1001,96 @@
         <v>17</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="J8" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="B9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="L8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="J9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="F10" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="L10" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="M10" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
   </sheetData>
@@ -1101,6 +1101,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="53c3d528-01ed-4c74-89e9-ceef25cbeca4">
@@ -1109,15 +1118,6 @@
     <TaxCatchAll xmlns="f3c758c6-693a-4f90-9954-357349518af8" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1364,20 +1364,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45B7021C-8291-4B90-8061-712C4E6F7AD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158BE85B-2F58-4DEF-B9C8-8618EFE76EE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="53c3d528-01ed-4c74-89e9-ceef25cbeca4"/>
     <ds:schemaRef ds:uri="f3c758c6-693a-4f90-9954-357349518af8"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{45B7021C-8291-4B90-8061-712C4E6F7AD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>